<commit_message>
[12.0][FIX] added %10 and %20 tax rates to zirve excel report.
</commit_message>
<xml_diff>
--- a/altinkaya_excel_export/export_account_invoice_xlsx/gelir_fatura.xlsx
+++ b/altinkaya_excel_export/export_account_invoice_xlsx/gelir_fatura.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Tarih</t>
   </si>
@@ -43,10 +43,22 @@
     <t xml:space="preserve">KDV8</t>
   </si>
   <si>
+    <t xml:space="preserve">Matrah 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KDV10</t>
+  </si>
+  <si>
     <t xml:space="preserve">Matrah 18</t>
   </si>
   <si>
     <t xml:space="preserve">KDV 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matrah 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KDV 20</t>
   </si>
   <si>
     <t xml:space="preserve">Matrah</t>
@@ -228,19 +240,36 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IU1"/>
+  <dimension ref="A1:IY1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U7" activeCellId="0" sqref="U7"/>
+      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="9.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="7.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="5.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="10.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="6.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="10.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -280,34 +309,42 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
+      <c r="U1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="Y1" s="6"/>
       <c r="Z1" s="6"/>
       <c r="AA1" s="6"/>
@@ -539,6 +576,10 @@
       <c r="IS1" s="6"/>
       <c r="IT1" s="6"/>
       <c r="IU1" s="6"/>
+      <c r="IV1" s="6"/>
+      <c r="IW1" s="6"/>
+      <c r="IX1" s="6"/>
+      <c r="IY1" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>